<commit_message>
scripting for olt from upstream
</commit_message>
<xml_diff>
--- a/Gaurav_MyLearning/NewLearning/iperf-3.17.1-win64/Logs/Line_Chart_Of_ZX_5G_DXB_2.4G.xlsx
+++ b/Gaurav_MyLearning/NewLearning/iperf-3.17.1-win64/Logs/Line_Chart_Of_ZX_5G_DXB_2.4G.xlsx
@@ -288,11 +288,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="134088960"/>
-        <c:axId val="134111232"/>
+        <c:axId val="131471616"/>
+        <c:axId val="131489792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="134088960"/>
+        <c:axId val="131471616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -300,14 +300,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134111232"/>
+        <c:crossAx val="131489792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134111232"/>
+        <c:axId val="131489792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -315,7 +315,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="134088960"/>
+        <c:crossAx val="131471616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -512,11 +512,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="134964736"/>
-        <c:axId val="134966272"/>
+        <c:axId val="132208128"/>
+        <c:axId val="132209664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="134964736"/>
+        <c:axId val="132208128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -524,14 +524,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134966272"/>
+        <c:crossAx val="132209664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134966272"/>
+        <c:axId val="132209664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -539,7 +539,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="134964736"/>
+        <c:crossAx val="132208128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -735,11 +735,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="136247936"/>
-        <c:axId val="136266112"/>
+        <c:axId val="134875776"/>
+        <c:axId val="134885760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="136247936"/>
+        <c:axId val="134875776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -747,14 +747,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136266112"/>
+        <c:crossAx val="134885760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136266112"/>
+        <c:axId val="134885760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -762,7 +762,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="136247936"/>
+        <c:crossAx val="134875776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>